<commit_message>
DataCamp - Importing Data
</commit_message>
<xml_diff>
--- a/pystudy/data/pop_growth.xlsx
+++ b/pystudy/data/pop_growth.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28016"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/woosa7/Documents/PythonDataAnalytics/pystudy/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Github\PythonDataAnalytics\pystudy\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{205073D3-51F7-4A05-BD6B-EA01C860818D}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14740" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="25605" windowHeight="14745" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="before2000" sheetId="1" r:id="rId1"/>
@@ -43,7 +44,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -85,13 +86,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="기본" xfId="0" builtinId="0"/>
+    <cellStyle name="표준" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -359,16 +363,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="18" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="17.25" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -376,7 +380,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>2.5299999999999998</v>
       </c>
@@ -384,7 +388,7 @@
         <v>1950</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2.57</v>
       </c>
@@ -392,7 +396,7 @@
         <v>1951</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>2.62</v>
       </c>
@@ -400,7 +404,7 @@
         <v>1952</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>2.67</v>
       </c>
@@ -408,7 +412,7 @@
         <v>1953</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>2.71</v>
       </c>
@@ -416,7 +420,7 @@
         <v>1954</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>2.76</v>
       </c>
@@ -424,7 +428,7 @@
         <v>1955</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>2.81</v>
       </c>
@@ -432,7 +436,7 @@
         <v>1956</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>2.86</v>
       </c>
@@ -440,7 +444,7 @@
         <v>1957</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>2.92</v>
       </c>
@@ -448,7 +452,7 @@
         <v>1958</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>2.97</v>
       </c>
@@ -456,7 +460,7 @@
         <v>1959</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>3.03</v>
       </c>
@@ -464,7 +468,7 @@
         <v>1960</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>3.08</v>
       </c>
@@ -472,7 +476,7 @@
         <v>1961</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>3.14</v>
       </c>
@@ -480,7 +484,7 @@
         <v>1962</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>3.2</v>
       </c>
@@ -488,7 +492,7 @@
         <v>1963</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>3.26</v>
       </c>
@@ -496,7 +500,7 @@
         <v>1964</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>3.33</v>
       </c>
@@ -504,7 +508,7 @@
         <v>1965</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>3.4</v>
       </c>
@@ -512,7 +516,7 @@
         <v>1966</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>3.47</v>
       </c>
@@ -520,7 +524,7 @@
         <v>1967</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>3.54</v>
       </c>
@@ -528,7 +532,7 @@
         <v>1968</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>3.62</v>
       </c>
@@ -536,7 +540,7 @@
         <v>1969</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>3.69</v>
       </c>
@@ -544,7 +548,7 @@
         <v>1970</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>3.77</v>
       </c>
@@ -552,7 +556,7 @@
         <v>1971</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>3.84</v>
       </c>
@@ -560,7 +564,7 @@
         <v>1972</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>3.92</v>
       </c>
@@ -568,7 +572,7 @@
         <v>1973</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>4</v>
       </c>
@@ -576,7 +580,7 @@
         <v>1974</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>4.07</v>
       </c>
@@ -584,7 +588,7 @@
         <v>1975</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>4.1500000000000004</v>
       </c>
@@ -592,7 +596,7 @@
         <v>1976</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>4.22</v>
       </c>
@@ -600,7 +604,7 @@
         <v>1977</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>4.3</v>
       </c>
@@ -608,7 +612,7 @@
         <v>1978</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>4.37</v>
       </c>
@@ -616,7 +620,7 @@
         <v>1979</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>4.45</v>
       </c>
@@ -624,7 +628,7 @@
         <v>1980</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>4.53</v>
       </c>
@@ -632,7 +636,7 @@
         <v>1981</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>4.6100000000000003</v>
       </c>
@@ -640,7 +644,7 @@
         <v>1982</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>4.6900000000000004</v>
       </c>
@@ -648,7 +652,7 @@
         <v>1983</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>4.78</v>
       </c>
@@ -656,7 +660,7 @@
         <v>1984</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>4.8600000000000003</v>
       </c>
@@ -664,7 +668,7 @@
         <v>1985</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>4.95</v>
       </c>
@@ -672,7 +676,7 @@
         <v>1986</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>5.05</v>
       </c>
@@ -680,7 +684,7 @@
         <v>1987</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>5.14</v>
       </c>
@@ -688,7 +692,7 @@
         <v>1988</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>5.23</v>
       </c>
@@ -696,7 +700,7 @@
         <v>1989</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>5.32</v>
       </c>
@@ -704,7 +708,7 @@
         <v>1990</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>5.41</v>
       </c>
@@ -712,7 +716,7 @@
         <v>1991</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>5.49</v>
       </c>
@@ -720,7 +724,7 @@
         <v>1992</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>5.58</v>
       </c>
@@ -728,7 +732,7 @@
         <v>1993</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>5.66</v>
       </c>
@@ -736,7 +740,7 @@
         <v>1994</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>5.74</v>
       </c>
@@ -744,7 +748,7 @@
         <v>1995</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>5.82</v>
       </c>
@@ -752,7 +756,7 @@
         <v>1996</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>5.9</v>
       </c>
@@ -760,7 +764,7 @@
         <v>1997</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>5.98</v>
       </c>
@@ -768,7 +772,7 @@
         <v>1998</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>6.05</v>
       </c>
@@ -783,16 +787,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B102"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="18" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="17.25" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -800,7 +802,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>6.13</v>
       </c>
@@ -808,7 +810,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>6.2</v>
       </c>
@@ -816,7 +818,7 @@
         <v>2001</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>6.28</v>
       </c>
@@ -824,7 +826,7 @@
         <v>2002</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>6.36</v>
       </c>
@@ -832,7 +834,7 @@
         <v>2003</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>6.44</v>
       </c>
@@ -840,7 +842,7 @@
         <v>2004</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6.51</v>
       </c>
@@ -848,7 +850,7 @@
         <v>2005</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>6.59</v>
       </c>
@@ -856,7 +858,7 @@
         <v>2006</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>6.67</v>
       </c>
@@ -864,7 +866,7 @@
         <v>2007</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>6.75</v>
       </c>
@@ -872,7 +874,7 @@
         <v>2008</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>6.83</v>
       </c>
@@ -880,7 +882,7 @@
         <v>2009</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>6.92</v>
       </c>
@@ -888,7 +890,7 @@
         <v>2010</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>7</v>
       </c>
@@ -896,7 +898,7 @@
         <v>2011</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>7.08</v>
       </c>
@@ -904,7 +906,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>7.16</v>
       </c>
@@ -912,7 +914,7 @@
         <v>2013</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>7.24</v>
       </c>
@@ -920,7 +922,7 @@
         <v>2014</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>7.32</v>
       </c>
@@ -928,7 +930,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>7.4</v>
       </c>
@@ -936,7 +938,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>7.48</v>
       </c>
@@ -944,7 +946,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>7.56</v>
       </c>
@@ -952,7 +954,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>7.64</v>
       </c>
@@ -960,7 +962,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>7.72</v>
       </c>
@@ -968,7 +970,7 @@
         <v>2020</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>7.79</v>
       </c>
@@ -976,7 +978,7 @@
         <v>2021</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>7.87</v>
       </c>
@@ -984,7 +986,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>7.94</v>
       </c>
@@ -992,7 +994,7 @@
         <v>2023</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>8.01</v>
       </c>
@@ -1000,7 +1002,7 @@
         <v>2024</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>8.08</v>
       </c>
@@ -1008,7 +1010,7 @@
         <v>2025</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>8.15</v>
       </c>
@@ -1016,7 +1018,7 @@
         <v>2026</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>8.2200000000000006</v>
       </c>
@@ -1024,7 +1026,7 @@
         <v>2027</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>8.2899999999999991</v>
       </c>
@@ -1032,7 +1034,7 @@
         <v>2028</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>8.36</v>
       </c>
@@ -1040,7 +1042,7 @@
         <v>2029</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>8.42</v>
       </c>
@@ -1048,7 +1050,7 @@
         <v>2030</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>8.49</v>
       </c>
@@ -1056,7 +1058,7 @@
         <v>2031</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>8.56</v>
       </c>
@@ -1064,7 +1066,7 @@
         <v>2032</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>8.6199999999999992</v>
       </c>
@@ -1072,7 +1074,7 @@
         <v>2033</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>8.68</v>
       </c>
@@ -1080,7 +1082,7 @@
         <v>2034</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>8.74</v>
       </c>
@@ -1088,7 +1090,7 @@
         <v>2035</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>8.8000000000000007</v>
       </c>
@@ -1096,7 +1098,7 @@
         <v>2036</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>8.86</v>
       </c>
@@ -1104,7 +1106,7 @@
         <v>2037</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>8.92</v>
       </c>
@@ -1112,7 +1114,7 @@
         <v>2038</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>8.98</v>
       </c>
@@ -1120,7 +1122,7 @@
         <v>2039</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>9.0399999999999991</v>
       </c>
@@ -1128,7 +1130,7 @@
         <v>2040</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>9.09</v>
       </c>
@@ -1136,7 +1138,7 @@
         <v>2041</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>9.15</v>
       </c>
@@ -1144,7 +1146,7 @@
         <v>2042</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>9.1999999999999993</v>
       </c>
@@ -1152,7 +1154,7 @@
         <v>2043</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>9.26</v>
       </c>
@@ -1160,7 +1162,7 @@
         <v>2044</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>9.31</v>
       </c>
@@ -1168,7 +1170,7 @@
         <v>2045</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>9.36</v>
       </c>
@@ -1176,7 +1178,7 @@
         <v>2046</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>9.41</v>
       </c>
@@ -1184,7 +1186,7 @@
         <v>2047</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>9.4600000000000009</v>
       </c>
@@ -1192,7 +1194,7 @@
         <v>2048</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>9.5</v>
       </c>
@@ -1200,7 +1202,7 @@
         <v>2049</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>9.5500000000000007</v>
       </c>
@@ -1208,7 +1210,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>9.6</v>
       </c>
@@ -1216,7 +1218,7 @@
         <v>2051</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>9.64</v>
       </c>
@@ -1224,7 +1226,7 @@
         <v>2052</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>9.68</v>
       </c>
@@ -1232,7 +1234,7 @@
         <v>2053</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A56">
         <v>9.73</v>
       </c>
@@ -1240,7 +1242,7 @@
         <v>2054</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A57">
         <v>9.77</v>
       </c>
@@ -1248,7 +1250,7 @@
         <v>2055</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A58">
         <v>9.81</v>
       </c>
@@ -1256,7 +1258,7 @@
         <v>2056</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A59">
         <v>9.85</v>
       </c>
@@ -1264,7 +1266,7 @@
         <v>2057</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A60">
         <v>9.8800000000000008</v>
       </c>
@@ -1272,7 +1274,7 @@
         <v>2058</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A61">
         <v>9.92</v>
       </c>
@@ -1280,7 +1282,7 @@
         <v>2059</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A62">
         <v>9.9600000000000009</v>
       </c>
@@ -1288,7 +1290,7 @@
         <v>2060</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A63">
         <v>9.99</v>
       </c>
@@ -1296,7 +1298,7 @@
         <v>2061</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A64">
         <v>10.029999999999999</v>
       </c>
@@ -1304,7 +1306,7 @@
         <v>2062</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A65">
         <v>10.06</v>
       </c>
@@ -1312,7 +1314,7 @@
         <v>2063</v>
       </c>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A66">
         <v>10.09</v>
       </c>
@@ -1320,7 +1322,7 @@
         <v>2064</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A67">
         <v>10.130000000000001</v>
       </c>
@@ -1328,7 +1330,7 @@
         <v>2065</v>
       </c>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A68">
         <v>10.16</v>
       </c>
@@ -1336,7 +1338,7 @@
         <v>2066</v>
       </c>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A69">
         <v>10.19</v>
       </c>
@@ -1344,7 +1346,7 @@
         <v>2067</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A70">
         <v>10.220000000000001</v>
       </c>
@@ -1352,7 +1354,7 @@
         <v>2068</v>
       </c>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A71">
         <v>10.25</v>
       </c>
@@ -1360,7 +1362,7 @@
         <v>2069</v>
       </c>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A72">
         <v>10.28</v>
       </c>
@@ -1368,7 +1370,7 @@
         <v>2070</v>
       </c>
     </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A73">
         <v>10.31</v>
       </c>
@@ -1376,7 +1378,7 @@
         <v>2071</v>
       </c>
     </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A74">
         <v>10.33</v>
       </c>
@@ -1384,7 +1386,7 @@
         <v>2072</v>
       </c>
     </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A75">
         <v>10.36</v>
       </c>
@@ -1392,7 +1394,7 @@
         <v>2073</v>
       </c>
     </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A76">
         <v>10.38</v>
       </c>
@@ -1400,7 +1402,7 @@
         <v>2074</v>
       </c>
     </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A77">
         <v>10.41</v>
       </c>
@@ -1408,7 +1410,7 @@
         <v>2075</v>
       </c>
     </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A78">
         <v>10.43</v>
       </c>
@@ -1416,7 +1418,7 @@
         <v>2076</v>
       </c>
     </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A79">
         <v>10.46</v>
       </c>
@@ -1424,7 +1426,7 @@
         <v>2077</v>
       </c>
     </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A80">
         <v>10.48</v>
       </c>
@@ -1432,7 +1434,7 @@
         <v>2078</v>
       </c>
     </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A81">
         <v>10.5</v>
       </c>
@@ -1440,7 +1442,7 @@
         <v>2079</v>
       </c>
     </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A82">
         <v>10.52</v>
       </c>
@@ -1448,7 +1450,7 @@
         <v>2080</v>
       </c>
     </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A83">
         <v>10.55</v>
       </c>
@@ -1456,7 +1458,7 @@
         <v>2081</v>
       </c>
     </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A84">
         <v>10.57</v>
       </c>
@@ -1464,7 +1466,7 @@
         <v>2082</v>
       </c>
     </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A85">
         <v>10.59</v>
       </c>
@@ -1472,7 +1474,7 @@
         <v>2083</v>
       </c>
     </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A86">
         <v>10.61</v>
       </c>
@@ -1480,7 +1482,7 @@
         <v>2084</v>
       </c>
     </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A87">
         <v>10.63</v>
       </c>
@@ -1488,7 +1490,7 @@
         <v>2085</v>
       </c>
     </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A88">
         <v>10.65</v>
       </c>
@@ -1496,7 +1498,7 @@
         <v>2086</v>
       </c>
     </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A89">
         <v>10.66</v>
       </c>
@@ -1504,7 +1506,7 @@
         <v>2087</v>
       </c>
     </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A90">
         <v>10.68</v>
       </c>
@@ -1512,7 +1514,7 @@
         <v>2088</v>
       </c>
     </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A91">
         <v>10.7</v>
       </c>
@@ -1520,7 +1522,7 @@
         <v>2089</v>
       </c>
     </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A92">
         <v>10.72</v>
       </c>
@@ -1528,7 +1530,7 @@
         <v>2090</v>
       </c>
     </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A93">
         <v>10.73</v>
       </c>
@@ -1536,7 +1538,7 @@
         <v>2091</v>
       </c>
     </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A94">
         <v>10.75</v>
       </c>
@@ -1544,7 +1546,7 @@
         <v>2092</v>
       </c>
     </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A95">
         <v>10.77</v>
       </c>
@@ -1552,7 +1554,7 @@
         <v>2093</v>
       </c>
     </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A96">
         <v>10.78</v>
       </c>
@@ -1560,7 +1562,7 @@
         <v>2094</v>
       </c>
     </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A97">
         <v>10.79</v>
       </c>
@@ -1568,7 +1570,7 @@
         <v>2095</v>
       </c>
     </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A98">
         <v>10.81</v>
       </c>
@@ -1576,7 +1578,7 @@
         <v>2096</v>
       </c>
     </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A99">
         <v>10.82</v>
       </c>
@@ -1584,7 +1586,7 @@
         <v>2097</v>
       </c>
     </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A100">
         <v>10.83</v>
       </c>
@@ -1592,7 +1594,7 @@
         <v>2098</v>
       </c>
     </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A101">
         <v>10.84</v>
       </c>
@@ -1600,7 +1602,7 @@
         <v>2099</v>
       </c>
     </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A102">
         <v>10.85</v>
       </c>
@@ -1611,5 +1613,6 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>